<commit_message>
Rerun falied cases implemented
</commit_message>
<xml_diff>
--- a/testData/Credentials.xlsx
+++ b/testData/Credentials.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2462007\Downloads\Identify_New_Bikes\Identify_New_Bikes\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA46DC65-DF7A-48D9-AE02-C47947B35035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0A352282-F2D8-4D5E-B5CF-0E160716BF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Google" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -387,10 +383,14 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>